<commit_message>
Performance measurements and plots for Rayleigh-Taylor 3D
</commit_message>
<xml_diff>
--- a/sheet05/data/Contest1ParallelPerformanceData.xlsx
+++ b/sheet05/data/Contest1ParallelPerformanceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tobias\MolSim-WS23-24\sheet05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281F5D82-1E4D-42B7-A6BB-D1F42B92EC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798D2329-9760-4C03-A80A-D301ACB15685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -269,12 +269,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -282,6 +280,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,13 +305,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -8079,8 +8077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8495,553 +8493,553 @@
     </row>
     <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="17"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="22"/>
     </row>
     <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="12" t="s">
+      <c r="D32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="12" t="s">
+      <c r="G32" s="18"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J32" s="13"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="12" t="s">
+      <c r="J32" s="18"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="M32" s="13"/>
-      <c r="N32" s="14"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="19"/>
     </row>
     <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G33" s="23" t="s">
+      <c r="G33" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="24" t="s">
+      <c r="H33" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="I33" s="18" t="s">
+      <c r="I33" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J33" s="19" t="s">
+      <c r="J33" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K33" s="20" t="s">
+      <c r="K33" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L33" s="23" t="s">
+      <c r="L33" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M33" s="23" t="s">
+      <c r="M33" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="N33" s="24" t="s">
+      <c r="N33" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="9">
+      <c r="B34" s="7">
         <v>1</v>
       </c>
       <c r="C34" s="2">
         <v>3.7440000000000002</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="1">
         <v>2670940.1709400001</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="3">
         <f>C$34/C34</f>
         <v>1</v>
       </c>
       <c r="F34" s="2">
         <v>3.7010000000000001</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="1">
         <v>2701972.4398810002</v>
       </c>
-      <c r="H34" s="5">
+      <c r="H34" s="3">
         <f>F$34/F34</f>
         <v>1</v>
       </c>
       <c r="I34" s="2">
         <v>3.6989999999999998</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="1">
         <v>2703433.3603679999</v>
       </c>
-      <c r="K34" s="5">
+      <c r="K34" s="3">
         <f>I$34/I34</f>
         <v>1</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34">
         <f>AVERAGE(C34,F34,I34)</f>
         <v>3.7146666666666666</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34">
         <f>AVERAGE(D34,G34,J34)</f>
         <v>2692115.3237296664</v>
       </c>
-      <c r="N34" s="5">
+      <c r="N34" s="3">
         <f>AVERAGE(E34,H34,K34)</f>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="10">
+      <c r="B35" s="8">
         <v>2</v>
       </c>
       <c r="C35" s="2">
         <v>2.9689999999999999</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="1">
         <v>3368137.4200070002</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="3">
         <f t="shared" ref="E35:E43" si="2">C$34/C35</f>
         <v>1.2610306500505222</v>
       </c>
       <c r="F35" s="2">
         <v>2.97</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="1">
         <v>3367003.3670029999</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H35" s="3">
         <f t="shared" ref="H35:H43" si="3">F$34/F35</f>
         <v>1.246127946127946</v>
       </c>
       <c r="I35" s="2">
         <v>2.9630000000000001</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="1">
         <v>3374957.8130270001</v>
       </c>
-      <c r="K35" s="5">
+      <c r="K35" s="3">
         <f t="shared" ref="K35:K43" si="4">I$34/I35</f>
         <v>1.248396895038812</v>
       </c>
-      <c r="L35" s="4">
-        <f>AVERAGE(C35,F35,I35)</f>
+      <c r="L35">
+        <f t="shared" ref="L35:L43" si="5">AVERAGE(C35,F35,I35)</f>
         <v>2.9673333333333338</v>
       </c>
-      <c r="M35" s="4">
-        <f>AVERAGE(D35,G35,J35)</f>
+      <c r="M35">
+        <f t="shared" ref="M35:M43" si="6">AVERAGE(D35,G35,J35)</f>
         <v>3370032.8666790002</v>
       </c>
-      <c r="N35" s="5">
-        <f t="shared" ref="N35:N43" si="5">AVERAGE(E35,H35,K35)</f>
+      <c r="N35" s="3">
+        <f t="shared" ref="N35:N43" si="7">AVERAGE(E35,H35,K35)</f>
         <v>1.25185183040576</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="10">
+      <c r="B36" s="8">
         <v>4</v>
       </c>
       <c r="C36" s="2">
         <v>2.1070000000000002</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="1">
         <v>4746084.480304</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="3">
         <f t="shared" si="2"/>
         <v>1.7769340294257236</v>
       </c>
       <c r="F36" s="2">
         <v>2.1150000000000002</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="1">
         <v>4728132.3877069997</v>
       </c>
-      <c r="H36" s="5">
+      <c r="H36" s="3">
         <f t="shared" si="3"/>
         <v>1.7498817966903071</v>
       </c>
       <c r="I36" s="2">
         <v>2.1240000000000001</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="1">
         <v>4708097.9284370001</v>
       </c>
-      <c r="K36" s="5">
+      <c r="K36" s="3">
         <f t="shared" si="4"/>
         <v>1.7415254237288134</v>
       </c>
-      <c r="L36" s="4">
-        <f>AVERAGE(C36,F36,I36)</f>
+      <c r="L36">
+        <f t="shared" si="5"/>
         <v>2.1153333333333335</v>
       </c>
-      <c r="M36" s="4">
-        <f>AVERAGE(D36,G36,J36)</f>
+      <c r="M36">
+        <f t="shared" si="6"/>
         <v>4727438.2654826669</v>
       </c>
-      <c r="N36" s="5">
-        <f t="shared" si="5"/>
+      <c r="N36" s="3">
+        <f t="shared" si="7"/>
         <v>1.7561137499482813</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="10">
+      <c r="B37" s="8">
         <v>8</v>
       </c>
       <c r="C37" s="2">
         <v>1.6970000000000001</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="1">
         <v>5892751.9151440002</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="3">
         <f t="shared" si="2"/>
         <v>2.206246317030053</v>
       </c>
       <c r="F37" s="2">
         <v>1.6819999999999999</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="1">
         <v>5945303.2104639998</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H37" s="3">
         <f t="shared" si="3"/>
         <v>2.2003567181926278</v>
       </c>
       <c r="I37" s="2">
         <v>1.6639999999999999</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="1">
         <v>6009615.3846150003</v>
       </c>
-      <c r="K37" s="5">
+      <c r="K37" s="3">
         <f t="shared" si="4"/>
         <v>2.2229567307692308</v>
       </c>
-      <c r="L37" s="4">
-        <f>AVERAGE(C37,F37,I37)</f>
+      <c r="L37">
+        <f t="shared" si="5"/>
         <v>1.681</v>
       </c>
-      <c r="M37" s="4">
-        <f>AVERAGE(D37,G37,J37)</f>
+      <c r="M37">
+        <f t="shared" si="6"/>
         <v>5949223.5034076674</v>
       </c>
-      <c r="N37" s="5">
-        <f t="shared" si="5"/>
+      <c r="N37" s="3">
+        <f t="shared" si="7"/>
         <v>2.2098532553306369</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="10">
+      <c r="B38" s="8">
         <v>16</v>
       </c>
       <c r="C38" s="2">
         <v>1.419</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="1">
         <v>7047216.3495420003</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="3">
         <f t="shared" si="2"/>
         <v>2.6384778012684991</v>
       </c>
       <c r="F38" s="2">
         <v>1.4470000000000001</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="1">
         <v>6910850.034554</v>
       </c>
-      <c r="H38" s="5">
+      <c r="H38" s="3">
         <f t="shared" si="3"/>
         <v>2.5577055977885279</v>
       </c>
       <c r="I38" s="2">
         <v>1.42</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="1">
         <v>7042253.5211270005</v>
       </c>
-      <c r="K38" s="5">
+      <c r="K38" s="3">
         <f t="shared" si="4"/>
         <v>2.6049295774647887</v>
       </c>
-      <c r="L38" s="4">
-        <f>AVERAGE(C38,F38,I38)</f>
+      <c r="L38">
+        <f t="shared" si="5"/>
         <v>1.4286666666666665</v>
       </c>
-      <c r="M38" s="4">
-        <f>AVERAGE(D38,G38,J38)</f>
+      <c r="M38">
+        <f t="shared" si="6"/>
         <v>7000106.6350743333</v>
       </c>
-      <c r="N38" s="5">
-        <f t="shared" si="5"/>
+      <c r="N38" s="3">
+        <f t="shared" si="7"/>
         <v>2.6003709921739389</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="10">
+      <c r="B39" s="8">
         <v>28</v>
       </c>
       <c r="C39" s="2">
         <v>1.359</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="1">
         <v>7358351.7292130003</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="3">
         <f t="shared" si="2"/>
         <v>2.7549668874172188</v>
       </c>
       <c r="F39" s="2">
         <v>1.331</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="1">
         <v>7513148.0090159997</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H39" s="3">
         <f t="shared" si="3"/>
         <v>2.7806160781367395</v>
       </c>
       <c r="I39" s="2">
         <v>1.3160000000000001</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="1">
         <v>7598784.1945289997</v>
       </c>
-      <c r="K39" s="5">
+      <c r="K39" s="3">
         <f t="shared" si="4"/>
         <v>2.8107902735562309</v>
       </c>
-      <c r="L39" s="4">
-        <f>AVERAGE(C39,F39,I39)</f>
+      <c r="L39">
+        <f t="shared" si="5"/>
         <v>1.3353333333333335</v>
       </c>
-      <c r="M39" s="4">
-        <f>AVERAGE(D39,G39,J39)</f>
+      <c r="M39">
+        <f t="shared" si="6"/>
         <v>7490094.6442526663</v>
       </c>
-      <c r="N39" s="5">
-        <f t="shared" si="5"/>
+      <c r="N39" s="3">
+        <f t="shared" si="7"/>
         <v>2.7821244130367297</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="10">
+      <c r="B40" s="8">
         <v>42</v>
       </c>
       <c r="C40" s="2">
         <v>1.3240000000000001</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="1">
         <v>7552870.0906339996</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="3">
         <f t="shared" si="2"/>
         <v>2.8277945619335347</v>
       </c>
       <c r="F40" s="2">
         <v>1.29</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="1">
         <v>7751937.9844960002</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H40" s="3">
         <f t="shared" si="3"/>
         <v>2.8689922480620154</v>
       </c>
       <c r="I40" s="2">
         <v>1.304</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="1">
         <v>7668711.6564419996</v>
       </c>
-      <c r="K40" s="5">
+      <c r="K40" s="3">
         <f t="shared" si="4"/>
         <v>2.8366564417177913</v>
       </c>
-      <c r="L40" s="4">
-        <f>AVERAGE(C40,F40,I40)</f>
+      <c r="L40">
+        <f t="shared" si="5"/>
         <v>1.306</v>
       </c>
-      <c r="M40" s="4">
-        <f>AVERAGE(D40,G40,J40)</f>
+      <c r="M40">
+        <f t="shared" si="6"/>
         <v>7657839.9105240004</v>
       </c>
-      <c r="N40" s="5">
-        <f t="shared" si="5"/>
+      <c r="N40" s="3">
+        <f t="shared" si="7"/>
         <v>2.8444810839044474</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="10">
+      <c r="B41" s="8">
         <v>56</v>
       </c>
       <c r="C41" s="2">
         <v>1.915</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="1">
         <v>5221932.114883</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="3">
         <f t="shared" si="2"/>
         <v>1.9550913838120105</v>
       </c>
       <c r="F41" s="2">
         <v>1.8360000000000001</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="1">
         <v>5446623.0936820004</v>
       </c>
-      <c r="H41" s="5">
+      <c r="H41" s="3">
         <f t="shared" si="3"/>
         <v>2.0157952069716774</v>
       </c>
       <c r="I41" s="2">
         <v>4.4160000000000004</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="1">
         <v>2264492.7536229999</v>
       </c>
-      <c r="K41" s="5">
+      <c r="K41" s="3">
         <f t="shared" si="4"/>
         <v>0.83763586956521729</v>
       </c>
-      <c r="L41" s="4">
-        <f>AVERAGE(C41,F41,I41)</f>
+      <c r="L41">
+        <f t="shared" si="5"/>
         <v>2.7223333333333337</v>
       </c>
-      <c r="M41" s="4">
-        <f>AVERAGE(D41,G41,J41)</f>
+      <c r="M41">
+        <f t="shared" si="6"/>
         <v>4311015.987396</v>
       </c>
-      <c r="N41" s="5">
-        <f t="shared" si="5"/>
+      <c r="N41" s="3">
+        <f t="shared" si="7"/>
         <v>1.6028408201163018</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="10">
+      <c r="B42" s="8">
         <v>72</v>
       </c>
       <c r="C42" s="2">
         <v>5.335</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="1">
         <v>1874414.2455480001</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="3">
         <f t="shared" si="2"/>
         <v>0.70178069353327088</v>
       </c>
       <c r="F42" s="2">
         <v>1.9930000000000001</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="1">
         <v>5017561.4651279999</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="3">
         <f t="shared" si="3"/>
         <v>1.8569994982438534</v>
       </c>
       <c r="I42" s="2">
         <v>8.6</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="1">
         <v>1162790.6976739999</v>
       </c>
-      <c r="K42" s="5">
+      <c r="K42" s="3">
         <f t="shared" si="4"/>
         <v>0.43011627906976746</v>
       </c>
-      <c r="L42" s="4">
-        <f>AVERAGE(C42,F42,I42)</f>
+      <c r="L42">
+        <f t="shared" si="5"/>
         <v>5.3093333333333339</v>
       </c>
-      <c r="M42" s="4">
-        <f>AVERAGE(D42,G42,J42)</f>
+      <c r="M42">
+        <f t="shared" si="6"/>
         <v>2684922.1361166663</v>
       </c>
-      <c r="N42" s="5">
-        <f t="shared" si="5"/>
+      <c r="N42" s="3">
+        <f t="shared" si="7"/>
         <v>0.9962988236156306</v>
       </c>
     </row>
     <row r="43" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="11">
+      <c r="B43" s="9">
         <v>96</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="4">
         <v>35.875999999999998</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="5">
         <v>278737.87490200001</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="6">
         <f t="shared" si="2"/>
         <v>0.1043594603634742</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="4">
         <v>10.127000000000001</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G43" s="5">
         <v>987459.26730499999</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H43" s="6">
         <f t="shared" si="3"/>
         <v>0.36545867482966327</v>
       </c>
-      <c r="I43" s="6">
+      <c r="I43" s="4">
         <v>10.798</v>
       </c>
-      <c r="J43" s="7">
+      <c r="J43" s="5">
         <v>926097.42544899997</v>
       </c>
-      <c r="K43" s="8">
+      <c r="K43" s="6">
         <f t="shared" si="4"/>
         <v>0.34256343767364328</v>
       </c>
-      <c r="L43" s="7">
-        <f>AVERAGE(C43,F43,I43)</f>
+      <c r="L43" s="5">
+        <f t="shared" si="5"/>
         <v>18.933666666666667</v>
       </c>
-      <c r="M43" s="7">
-        <f>AVERAGE(D43,G43,J43)</f>
+      <c r="M43" s="5">
+        <f t="shared" si="6"/>
         <v>730764.85588533338</v>
       </c>
-      <c r="N43" s="8">
-        <f t="shared" si="5"/>
+      <c r="N43" s="6">
+        <f t="shared" si="7"/>
         <v>0.27079385762226021</v>
       </c>
     </row>

</xml_diff>